<commit_message>
Dodano pełny schemat działania dla układu 3x3
</commit_message>
<xml_diff>
--- a/SI schematics/3x3.xlsx
+++ b/SI schematics/3x3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubat\Documents\projekt-zaliczenie-npg\SI schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDEBCA7-3791-4634-AE01-0492B4B6DFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7D813E-0919-43A4-A702-C1B3EF787C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8949F19C-7FE2-47A5-9C94-C8B26AFA58F0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8949F19C-7FE2-47A5-9C94-C8B26AFA58F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Move 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="2">
   <si>
     <t>X</t>
   </si>
@@ -60,7 +60,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +76,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,12 +113,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1251,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A856E1-C18D-4B5C-BDE8-280C966DF13A}">
   <dimension ref="A1:S139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="K143" sqref="K143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5154,12 +5161,3490 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C28D61-CFC2-4D43-9CF9-8E6E71ACF33E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K171"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="I10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="I23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="I34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="3"/>
+      <c r="E82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G82" s="2"/>
+      <c r="I82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="E91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G91" s="2"/>
+      <c r="I91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="E95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="E97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="E99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1"/>
+      <c r="I99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="E103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1"/>
+      <c r="I103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1"/>
+      <c r="I111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="E115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="E119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G119" s="1"/>
+      <c r="I119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K125" s="2"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A126" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" s="2"/>
+      <c r="E127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G127" s="1"/>
+      <c r="I127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G129" s="1"/>
+      <c r="I129" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K129" s="2"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" s="2"/>
+      <c r="E130" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K131" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K133" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I134" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K134" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135" s="1"/>
+      <c r="E135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G135" s="2"/>
+      <c r="I135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J135" s="2"/>
+      <c r="K135" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" s="1"/>
+      <c r="E139" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G139" s="1"/>
+      <c r="I139" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K141" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K142" s="2"/>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="1"/>
+      <c r="E143" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G143" s="2"/>
+      <c r="I143" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J143" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K143" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K146" s="1"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K147" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K149" s="1"/>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I151" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I153" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="2"/>
+      <c r="B154" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I154" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J154" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K154" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I155" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J155" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K155" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I158" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I159" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K159" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A161" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="E161" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I161" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G162" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K162" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I163" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J163" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A165" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G165" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J165" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K165" s="1"/>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G166" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A167" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A169" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B169" s="2"/>
+      <c r="C169" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G169" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A170" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G170" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A171" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Poprawiono pełny schemat działania dla układu 3x3
</commit_message>
<xml_diff>
--- a/SI schematics/3x3.xlsx
+++ b/SI schematics/3x3.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubat\Documents\projekt-zaliczenie-npg\SI schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7D813E-0919-43A4-A702-C1B3EF787C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794B6AA7-46AD-4A89-974B-81D7705F1ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8949F19C-7FE2-47A5-9C94-C8B26AFA58F0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{8949F19C-7FE2-47A5-9C94-C8B26AFA58F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Move 1" sheetId="1" r:id="rId1"/>
     <sheet name="Move 2" sheetId="2" r:id="rId2"/>
     <sheet name="Move 3" sheetId="3" r:id="rId3"/>
     <sheet name="Move 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Move 1SI" sheetId="5" r:id="rId5"/>
+    <sheet name="Move 2SI" sheetId="6" r:id="rId6"/>
+    <sheet name="Move 3SI" sheetId="7" r:id="rId7"/>
+    <sheet name="Move 4SI" sheetId="8" r:id="rId8"/>
+    <sheet name="Move 5SI" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="2">
   <si>
     <t>X</t>
   </si>
@@ -5163,7 +5168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C28D61-CFC2-4D43-9CF9-8E6E71ACF33E}">
   <dimension ref="A1:K171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
@@ -8647,4 +8652,2274 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3486AE-CA56-475B-94D4-CB0985881ABF}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1CFEF1-13DB-422A-ACD6-1C8B540B9CD7}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E160047-5317-4167-BA86-4E9C5D780D35}">
+  <dimension ref="A1:W31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29:K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="12" max="12" width="8.88671875" style="4"/>
+    <col min="16" max="16" width="8.88671875" style="4"/>
+    <col min="20" max="20" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="Q1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="U1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="U2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2"/>
+      <c r="U3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="U6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="U9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="U11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="U13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="Q14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="I15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="Q15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2"/>
+      <c r="U15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="U18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="E19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="Q19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="U19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="Q21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="U21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="I22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2"/>
+      <c r="U22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="I23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="Q23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2"/>
+      <c r="U23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="M27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="Q27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="U27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="Q29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="U29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="I30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="M30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="Q30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E4399F-4AC2-4597-A50F-5D596F9624CC}">
+  <dimension ref="A1:O31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="M21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="M23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F443FC-A85D-468C-B0FC-54DD5AE25043}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>